<commit_message>
Further updated bib and down to 8 pages!
</commit_message>
<xml_diff>
--- a/data/Results.xlsx
+++ b/data/Results.xlsx
@@ -8042,8 +8042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8219,16 +8219,16 @@
         <v>3.0019999999999999E-3</v>
       </c>
       <c r="E4">
-        <v>3.1605490000000001</v>
+        <v>3.4529580000000002</v>
       </c>
       <c r="F4">
-        <v>0.22569900000000001</v>
+        <v>0.213204</v>
       </c>
       <c r="G4">
-        <v>3.7941259999999999</v>
+        <v>3.1454659999999999</v>
       </c>
       <c r="H4">
-        <v>5.122153</v>
+        <v>6.2055899999999999</v>
       </c>
       <c r="J4">
         <v>0.5</v>
@@ -8237,28 +8237,28 @@
         <v>0.5</v>
       </c>
       <c r="L4">
-        <v>0.887656</v>
+        <v>0.788937</v>
       </c>
       <c r="M4">
-        <v>0.76726899999999998</v>
+        <v>0.70854200000000001</v>
       </c>
       <c r="N4">
-        <v>0.76212199999999997</v>
+        <v>0.78182300000000005</v>
       </c>
       <c r="O4">
-        <v>0.732074</v>
+        <v>0.76264299999999996</v>
       </c>
       <c r="Q4">
-        <v>2560631.4593409998</v>
+        <v>2093263.2566800001</v>
       </c>
       <c r="R4">
-        <v>2550279.5662949998</v>
+        <v>2847983.4667079998</v>
       </c>
       <c r="S4">
-        <v>2787312.008841</v>
+        <v>2159244.042963</v>
       </c>
       <c r="T4">
-        <v>1623132.096315</v>
+        <v>1640505.47233</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>